<commit_message>
Refatoracao diagrama de caso de uso
</commit_message>
<xml_diff>
--- a/Documentacao/Documentacao/PlanilhaDeAlertas.xlsx
+++ b/Documentacao/Documentacao/PlanilhaDeAlertas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projeto de PI\Project2nd\Documentacao\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\GetGame\Documentacao\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,15 +96,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDF7F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -112,28 +124,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -142,6 +286,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFDF7F"/>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -463,13 +613,6 @@
     <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
@@ -477,126 +620,131 @@
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="3">
         <v>0.96</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="16">
         <v>0.81</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D15" s="18">
         <v>0.81</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" s="10" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C11:E11"/>
+  <mergeCells count="1">
+    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>